<commit_message>
updation in import section and menu
</commit_message>
<xml_diff>
--- a/public/images/Sample_File.xlsx
+++ b/public/images/Sample_File.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="30">
   <si>
     <t>id</t>
   </si>
@@ -50,6 +50,60 @@
   </si>
   <si>
     <t>test@gmail.com</t>
+  </si>
+  <si>
+    <t>dob</t>
+  </si>
+  <si>
+    <t>23/1/2023</t>
+  </si>
+  <si>
+    <t>31/12/2022</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>100/1 rajwada,raipur</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>pincode</t>
+  </si>
+  <si>
+    <t>company</t>
+  </si>
+  <si>
+    <t>department</t>
+  </si>
+  <si>
+    <t>designation</t>
+  </si>
+  <si>
+    <t>others</t>
+  </si>
+  <si>
+    <t>Chhattisgarh</t>
+  </si>
+  <si>
+    <t>raipur</t>
+  </si>
+  <si>
+    <t>company name</t>
+  </si>
+  <si>
+    <t>department name</t>
+  </si>
+  <si>
+    <t>post</t>
+  </si>
+  <si>
+    <t>abc</t>
   </si>
 </sst>
 </file>
@@ -83,8 +137,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -381,10 +436,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="M3" sqref="M3:M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -392,9 +447,15 @@
     <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -407,8 +468,35 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:13">
       <c r="A2">
         <v>1</v>
       </c>
@@ -421,8 +509,35 @@
       <c r="D2" t="s">
         <v>5</v>
       </c>
+      <c r="E2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2">
+        <v>12345</v>
+      </c>
+      <c r="J2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M2" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:13">
       <c r="A3">
         <v>2</v>
       </c>
@@ -435,8 +550,35 @@
       <c r="D3" t="s">
         <v>7</v>
       </c>
+      <c r="E3" s="1">
+        <v>44571</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3">
+        <v>12345</v>
+      </c>
+      <c r="J3" t="s">
+        <v>26</v>
+      </c>
+      <c r="K3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L3" t="s">
+        <v>28</v>
+      </c>
+      <c r="M3" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:13">
       <c r="A4">
         <v>3</v>
       </c>
@@ -449,8 +591,35 @@
       <c r="D4" t="s">
         <v>9</v>
       </c>
+      <c r="E4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4">
+        <v>12345</v>
+      </c>
+      <c r="J4" t="s">
+        <v>26</v>
+      </c>
+      <c r="K4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M4" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:13">
       <c r="A5">
         <v>4</v>
       </c>
@@ -462,6 +631,33 @@
       </c>
       <c r="D5" t="s">
         <v>11</v>
+      </c>
+      <c r="E5" s="1">
+        <v>44927</v>
+      </c>
+      <c r="F5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5">
+        <v>12345</v>
+      </c>
+      <c r="J5" t="s">
+        <v>26</v>
+      </c>
+      <c r="K5" t="s">
+        <v>27</v>
+      </c>
+      <c r="L5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M5" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>